<commit_message>
Finalise adding my content
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -1,31 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bblack\switchdrive\git\curriculum-vitae\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C985AD6-7CC3-4A44-8F15-A6DB872342F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87EC8D9-F051-47B9-8178-A5C1D09D858F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" r:id="rId1"/>
     <sheet name="profil" sheetId="10" r:id="rId2"/>
-    <sheet name="skills" sheetId="2" r:id="rId3"/>
-    <sheet name="education" sheetId="3" r:id="rId4"/>
-    <sheet name="experience" sheetId="4" r:id="rId5"/>
-    <sheet name="workshop" sheetId="5" r:id="rId6"/>
-    <sheet name="packages" sheetId="6" r:id="rId7"/>
-    <sheet name="awards" sheetId="7" r:id="rId8"/>
-    <sheet name="oral" sheetId="8" r:id="rId9"/>
-    <sheet name="poster" sheetId="9" r:id="rId10"/>
+    <sheet name="languages" sheetId="11" r:id="rId3"/>
+    <sheet name="skills" sheetId="2" r:id="rId4"/>
+    <sheet name="education" sheetId="3" r:id="rId5"/>
+    <sheet name="experience" sheetId="4" r:id="rId6"/>
+    <sheet name="workshop" sheetId="5" r:id="rId7"/>
+    <sheet name="packages" sheetId="6" r:id="rId8"/>
+    <sheet name="awards" sheetId="7" r:id="rId9"/>
+    <sheet name="oral" sheetId="8" r:id="rId10"/>
+    <sheet name="poster" sheetId="9" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">poster!$A$1:$E$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">poster!$A$1:$E$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <webPublishing allowPng="1" targetScreenSize="1024x768" codePage="65001"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="190">
   <si>
     <t>position</t>
   </si>
@@ -176,22 +177,6 @@
   </si>
   <si>
     <t>2013-04</t>
-  </si>
-  <si>
-    <t>Lund, Sweden</t>
-  </si>
-  <si>
-    <t>Jan. 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Paris, France</t>
-  </si>
-  <si>
-    <t>Oct. 2018</t>
-  </si>
-  <si>
-    <t>Feb. 2016</t>
   </si>
   <si>
     <t>"Variants Génétiques Associés à la Trajectoire de la Glycémie à Jeun et à l’Incidence du Diabète de Type 2: Une Approche par Modèle Joint" (CA-075)</t>
@@ -292,12 +277,6 @@
     <t>Contributor</t>
   </si>
   <si>
-    <t>Longitudinal Genetic Modelling: Revisiting Associations of SNPs Associated With Blood Fasting Glucose in Normoglycemic Individuals</t>
-  </si>
-  <si>
-    <t>Jointly Modelling SNPs With Survival &amp; Longitudinal Trait</t>
-  </si>
-  <si>
     <t>Author / Creator</t>
   </si>
   <si>
@@ -338,57 +317,7 @@
     <t>CSS</t>
   </si>
   <si>
-    <t>My Journey To Transparency And Reproducibility</t>
-  </si>
-  <si>
-    <t>My Journey To Transparency And Reproducibility (French)</t>
-  </si>
-  <si>
-    <t>Online (Lille, France)</t>
-  </si>
-  <si>
-    <t>Apr. 2021</t>
-  </si>
-  <si>
-    <t>"Débuter" avec R en Commençant par le Début ... (French)</t>
-  </si>
-  <si>
-    <t>Jan. 2021</t>
-  </si>
-  <si>
-    <t>[mickael.canouil.fr](https://mickael.canouil.fr/talk/jointly-modelling-snps-with-survival-longitudinal-trait/)</t>
-  </si>
-  <si>
-    <t>[mickael.canouil.fr](https://mickael.canouil.fr/talk/debuter-avec-r-en-commencant-par-le-debut-...-french/)</t>
-  </si>
-  <si>
-    <t>[mickael.canouil.fr](https://mickael.canouil.fr/talk/my-journey-to-transparency-and-reproducibility-french/)</t>
-  </si>
-  <si>
-    <t>[mickael.canouil.fr](https://mickael.canouil.fr/talk/my-journey-to-transparency-and-reproducibility/)</t>
-  </si>
-  <si>
     <t>website</t>
-  </si>
-  <si>
-    <t>A Statistical Seminar Applied on Type 2 Diabetes  
-(Host: Pr. Paul Franks)</t>
-  </si>
-  <si>
-    <t>R Lille ([rlille.fr](https://rlille.fr))</t>
-  </si>
-  <si>
-    <t>Min2Rien ([www.min2rien.fr](https://www.min2rien.fr))</t>
-  </si>
-  <si>
-    <t>Thematic Day "Statistic &amp; Genomic"  
-of the "Réseau Interdisciplinaire  
-autour de la Statistique"  
-(RIS) ([ris.cnrs.fr](https://ris.cnrs.fr/))</t>
-  </si>
-  <si>
-    <t>Statistical Methods for Post Genomic Data  
-(SMPGD) ([math.univ-lille1.fr/~celisse/SMPGD](https://math.univ-lille1.fr/~celisse/SMPGD))</t>
   </si>
   <si>
     <t>mastodon</t>
@@ -489,18 +418,9 @@
     <t>*Funded project under the SwissRE Biodiversity and Ecosystem Services Scenarios Modelling Initiative*</t>
   </si>
   <si>
-    <t>Awards: University medal (highest average mark on degree route); Lawrence Ho student prize; Dennis Aw award.</t>
-  </si>
-  <si>
-    <t>Award: Outstanding academic achievement (highest GPA in cohort: 4.00/4.00)</t>
-  </si>
-  <si>
     <t>Hungary, Greece, UK</t>
   </si>
   <si>
-    <t>[NASCENT-Peru website](https://plus.ethz.ch/research/forschungsprojekte/NASCENT-PERU.html)</t>
-  </si>
-  <si>
     <t>Biodiversity and SMART Intern</t>
   </si>
   <si>
@@ -511,13 +431,6 @@
   </si>
   <si>
     <t>Aug. 2019</t>
-  </si>
-  <si>
-    <t>Produced protected area species inventories in line with Darwin Core standards
-utilising OpenRefine, R scripting and API services to expedite the collection of external
-data from the IUCN, EDGE ranking and CITES.
-Assisted in the training of new community biodiversity rangers in the process of
-SMART data collection in the field.</t>
   </si>
   <si>
     <t>The Wildlife Conservation Society (WCS)</t>
@@ -533,13 +446,6 @@
     <t>Siem Reap, Cambodia</t>
   </si>
   <si>
-    <t>Coordinated safety and risk management as well as logistics for all centre activities
-including multi day field trips to remote locations in Cambodia and Vietnam.
-Medical ‘point person’, facilitated first aid training for staff.
-Performed pastoral role: ensuring student well-being, resolving group management
-issues and facilitating cultural adaptation.</t>
-  </si>
-  <si>
     <t>Jan. 2018</t>
   </si>
   <si>
@@ -561,14 +467,6 @@
     <t>June. 2017</t>
   </si>
   <si>
-    <t>Managed a diverse team (Bunong Indigenous minority, and Khmer) of 48 staff.
-Oversaw the operation of an ecotourism project receiving 4000+ visitors a year.
-Facilitated ongoing capacity building of staff and development of the volunteer program. 
-Compiled budgets, handled cash flow to staff and submitted detailed financial reports.
-Produced reports for the board of directors and Cambodian government.
-Developed relationships with other environmental and conservation organisations in the region.</t>
-  </si>
-  <si>
     <t>Reproducible Research with R and Quarto: Workflows for data, projects and publications</t>
   </si>
   <si>
@@ -581,17 +479,157 @@
     <t>Sep. 2024</t>
   </si>
   <si>
-    <t>https://github.com/blenback/R-for-Reproducible-Research</t>
-  </si>
-  <si>
-    <t>I am a PhD student currently working within the [**ValPar.CH project**](https://valpar.ch/index_de.php) as part of the research group Planning of Landscape Urban Systems (PLUS) at ETH Zürich.</t>
+    <t>Independent Consultant Srae Y Community ecotourism project</t>
+  </si>
+  <si>
+    <t>World Wide Fund for Nature (WWF)</t>
+  </si>
+  <si>
+    <t>Dec. 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Undertook site visits to assess the status of the project and prepared a report, detailing strategies to make the project operational and sustainable. Planned and delivered a series of training sessions to project staff and stakeholders from other communities engaged in ecotourism. </t>
+  </si>
+  <si>
+    <t>Volunteer Development Officer &amp; Conservation Support Assistant</t>
+  </si>
+  <si>
+    <t>Central Scotland</t>
+  </si>
+  <si>
+    <t>Apr. 2015</t>
+  </si>
+  <si>
+    <t>May 2013</t>
+  </si>
+  <si>
+    <t>The Conservation Volunteers (TCV)</t>
+  </si>
+  <si>
+    <t>Produced protected area species inventories in line with Darwin Core standards utilising OpenRefine, R scripting and API services to expedite the collection of external data from the IUCN, EDGE ranking and CITES. Assisted in the training of new community biodiversity rangers in the process of SMART data collection in the field.</t>
+  </si>
+  <si>
+    <t>Coordinated safety and risk management as well as logistics for all centre activities including multi day field trips to remote locations in Cambodia and Vietnam. Medical ‘point person’, facilitated first aid training for staff. Performed pastoral role: ensuring student well-being, resolving group management issues and facilitating cultural adaptation.</t>
+  </si>
+  <si>
+    <t>Managed a diverse team (Bunong Indigenous minority, and Khmer) of 48 staff. Oversaw the operation of an ecotourism project receiving 4000+ visitors a year. Facilitated ongoing capacity building of staff and development of the volunteer program. 
+Compiled budgets, handled cash flow to staff and submitted detailed financial reports. Produced reports for the board of directors and Cambodian government. Developed relationships with other environmental and conservation organisations in the region.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Planned, developed and delivered the Ochils Landscape Partnerships volunteering program and two TCV community health projects. Engaged with, and ensured the safety and wellbeing of a diverse cross section of volunteers, many with physical or mental disabilities as well as young adults/children.</t>
+  </si>
+  <si>
+    <t>awards</t>
+  </si>
+  <si>
+    <t>University medal (highest average mark on degree route); Lawrence Ho student prize; Dennis Aw award.</t>
+  </si>
+  <si>
+    <t>Outstanding academic achievement (highest GPA in cohort: 4.00/4.00)</t>
+  </si>
+  <si>
+    <t>Ex-ante identification of policy interventions to secure a functioning ecological infrastructure: A participatory Bayesian Network approach in Switzerland</t>
+  </si>
+  <si>
+    <t>3rd Ecosystem Services Partnership Europe Regional conference</t>
+  </si>
+  <si>
+    <t>Tartu, Estonia</t>
+  </si>
+  <si>
+    <t>Jun. 2019</t>
+  </si>
+  <si>
+    <t>https://blenback.github.io/presentations/2021_06_09_ESP/</t>
+  </si>
+  <si>
+    <t>https://github.com/blenback/R-for-Reproducible-Research/</t>
+  </si>
+  <si>
+    <t>https://plus.ethz.ch/research/forschungsprojekte/NASCENT-PERU.html/</t>
+  </si>
+  <si>
+    <t>link_type</t>
+  </si>
+  <si>
+    <t>Combining filter and embedded approaches to improve variable selection in land use change Cellular Automata models</t>
+  </si>
+  <si>
+    <t>11th International Environmental Modelling and Software Society conference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Brussels, Belgium</t>
+  </si>
+  <si>
+    <t>Jul. 2022</t>
+  </si>
+  <si>
+    <t>https://blenback.github.io/presentations/2022_07_01_IEMSs_model_pres/</t>
+  </si>
+  <si>
+    <t>https://blenback.github.io/presentations/2022_07_01_IEMSs_ValParCH_pres/</t>
+  </si>
+  <si>
+    <t>Characterising non-stationarity in predictive models of land use in Swiss mountain parks to inform scenarios for deliberative transformation</t>
+  </si>
+  <si>
+    <t>ValPar.CH: Integrating land use change, Ecosystem Service and Biodiversity modelling to simulate pathways for a functioning Ecological Infrastructure for Switzerland</t>
+  </si>
+  <si>
+    <t>International Mountain conference 2022</t>
+  </si>
+  <si>
+    <t>Innsbruck, Austria</t>
+  </si>
+  <si>
+    <t>Sep. 2022</t>
+  </si>
+  <si>
+    <t>https://blenback.github.io/presentations/2022_09_13_IMC/</t>
+  </si>
+  <si>
+    <t>Broadening the scope of future visions for nature positive futures in Peru</t>
+  </si>
+  <si>
+    <t>Swiss Re Institute Resilience Summit 2023</t>
+  </si>
+  <si>
+    <t>Nov. 2023</t>
+  </si>
+  <si>
+    <t>https://blenback.github.io/presentations/2023_11_30_SwissRE/</t>
+  </si>
+  <si>
+    <t>Dinamica EGO</t>
+  </si>
+  <si>
+    <t>Native</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Conversational</t>
+  </si>
+  <si>
+    <t>Khmer</t>
+  </si>
+  <si>
+    <t>I am a PhD student currently working within the [**ValPar.CH**](https://valpar.ch/index_de.php) and [**NASCENT-Peru**](https://nascent-peru.github.io/) projects as part of the research group Planning of Landscape Urban Systems (PLUS) at ETH Zürich.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -603,6 +641,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -629,12 +673,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -919,7 +967,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,10 +1002,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="G1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -969,45 +1017,45 @@
         <v>7</v>
       </c>
       <c r="K1" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="L1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="M1" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="G2" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="H2" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="I2" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="J2" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="M2" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1020,6 +1068,142 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.7109375" customWidth="1"/>
+    <col min="2" max="2" width="85" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" t="s">
+        <v>180</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E6" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="E2:I2" r:id="rId2" display="https://blenback.github.io/presentations/2021_06_09_ESP/" xr:uid="{91963DD6-E5D6-4B0A-B27F-4049C782886D}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{AA09F58A-6E59-4E5C-9B56-EE1D04E2B316}"/>
+    <hyperlink ref="E4" r:id="rId4" xr:uid="{A013CEAB-2FCD-4175-B64E-AFEFC4EBC399}"/>
+    <hyperlink ref="E5" r:id="rId5" xr:uid="{F9DCC59D-DB81-4C87-A54D-F105942D3BD7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -1038,7 +1222,7 @@
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1052,58 +1236,58 @@
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
         <v>58</v>
-      </c>
-      <c r="C2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
         <v>55</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1116,7 +1300,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,21 +1318,21 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1156,7 +1340,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1167,13 +1351,13 @@
     </row>
     <row r="4" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1181,13 +1365,13 @@
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1195,13 +1379,13 @@
     </row>
     <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1213,11 +1397,58 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564B4F75-4CC5-4155-A321-F49D8C4AE087}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,7 +1470,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1247,15 +1478,15 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1263,7 +1494,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1271,7 +1502,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1279,15 +1510,15 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1295,103 +1526,15 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
         <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="84.28515625" customWidth="1"/>
-    <col min="6" max="6" width="142.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1400,11 +1543,110 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="84.28515625" customWidth="1"/>
+    <col min="7" max="7" width="142.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,7 +1654,7 @@
     <col min="1" max="1" width="50" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="117.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1427,7 +1669,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E1" t="s">
@@ -1437,76 +1679,117 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F6" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D3" t="s">
-        <v>158</v>
-      </c>
-      <c r="E3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>160</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D4" t="s">
-        <v>163</v>
-      </c>
-      <c r="E4" t="s">
-        <v>164</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1538,19 +1821,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="D2" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1561,12 +1844,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="A8:G8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1614,7 +1897,7 @@
         <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
         <v>36</v>
@@ -1637,7 +1920,7 @@
         <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
         <v>36</v>
@@ -1660,7 +1943,7 @@
         <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
         <v>36</v>
@@ -1674,39 +1957,39 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
         <v>75</v>
-      </c>
-      <c r="B5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" t="s">
-        <v>80</v>
       </c>
       <c r="E5" t="s">
         <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
         <v>36</v>
@@ -1715,21 +1998,21 @@
         <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
         <v>36</v>
@@ -1738,7 +2021,7 @@
         <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1747,12 +2030,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1763,7 +2046,7 @@
     <col min="6" max="6" width="99.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1782,167 +2065,37 @@
       <c r="F1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>147</v>
+        <v>121</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G2" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{A344B0D7-2544-4885-B67B-FC3F61A73CFD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="54.7109375" customWidth="1"/>
-    <col min="2" max="2" width="85" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1" display="https://mickael.canouil.fr/talk/my-journey-to-transparency-and-reproducibility-french/" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="E7" r:id="rId2" display="https://mickael.canouil.fr/talk/my-journey-to-transparency-and-reproducibility/" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-</worksheet>
 </file>
</xml_diff>